<commit_message>
Herramienta de Gestión QA del Producto
Actualización de fechas
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_PPQA/HGQA/HGQA_V1.0_2015.xlsx
+++ b/Area_de_Proceso-_PPQA/HGQA/HGQA_V1.0_2015.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="14250" windowHeight="5730" tabRatio="642" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="14250" windowHeight="5730" tabRatio="642" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="14" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="199">
   <si>
     <t>Analista Responsable</t>
   </si>
@@ -2535,102 +2535,142 @@
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="32" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="36" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="32" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="36" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2640,46 +2680,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="31" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2692,22 +2692,61 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="55" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="34" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="49" fillId="24" borderId="13" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="49" fillId="24" borderId="34" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="34" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2718,45 +2757,6 @@
     </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="55" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="34" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="49" fillId="24" borderId="13" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="49" fillId="24" borderId="34" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="13" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="34" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2870,6 +2870,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3080,7 +3081,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3104,10 +3107,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.4</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.6</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3138,6 +3141,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3243,6 +3247,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3903,6 +3908,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3931,7 +3937,7 @@
                   <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4068,6 +4074,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4173,6 +4180,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4507,6 +4515,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4696,6 +4705,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7557,22 +7567,22 @@
     <row r="2" spans="1:8" s="56" customFormat="1" ht="48.75" customHeight="1">
       <c r="A2" s="34"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="217" t="s">
+      <c r="C2" s="209" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="218"/>
-      <c r="E2" s="219"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="211"/>
     </row>
     <row r="3" spans="1:8" s="56" customFormat="1">
       <c r="A3" s="34"/>
       <c r="B3" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="225" t="s">
+      <c r="C3" s="217" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="226"/>
-      <c r="E3" s="227"/>
+      <c r="D3" s="218"/>
+      <c r="E3" s="219"/>
     </row>
     <row r="4" spans="1:8" s="56" customFormat="1" ht="21.75" customHeight="1">
       <c r="A4" s="34"/>
@@ -7584,12 +7594,12 @@
     </row>
     <row r="5" spans="1:8" ht="24.75" customHeight="1">
       <c r="A5" s="34"/>
-      <c r="B5" s="220" t="s">
+      <c r="B5" s="212" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="221"/>
-      <c r="D5" s="221"/>
-      <c r="E5" s="222"/>
+      <c r="C5" s="213"/>
+      <c r="D5" s="213"/>
+      <c r="E5" s="214"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="34"/>
@@ -7612,10 +7622,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="86"/>
-      <c r="D8" s="223" t="s">
+      <c r="D8" s="215" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="224"/>
+      <c r="E8" s="216"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="34"/>
@@ -7630,10 +7640,10 @@
         <v>93</v>
       </c>
       <c r="C10" s="56"/>
-      <c r="D10" s="228" t="s">
+      <c r="D10" s="223" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="228"/>
+      <c r="E10" s="223"/>
     </row>
     <row r="11" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A11" s="34"/>
@@ -7648,10 +7658,10 @@
         <v>93</v>
       </c>
       <c r="C12" s="56"/>
-      <c r="D12" s="228" t="s">
+      <c r="D12" s="223" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="228"/>
+      <c r="E12" s="223"/>
     </row>
     <row r="13" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A13" s="34"/>
@@ -7666,10 +7676,10 @@
         <v>93</v>
       </c>
       <c r="C14" s="56"/>
-      <c r="D14" s="228" t="s">
+      <c r="D14" s="223" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="228"/>
+      <c r="E14" s="223"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="32"/>
@@ -7684,10 +7694,10 @@
         <v>93</v>
       </c>
       <c r="C16" s="56"/>
-      <c r="D16" s="228" t="s">
+      <c r="D16" s="223" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="228"/>
+      <c r="E16" s="223"/>
       <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" s="47" customFormat="1" ht="12" customHeight="1">
@@ -7701,62 +7711,62 @@
       <c r="A18" s="32"/>
     </row>
     <row r="19" spans="1:8" s="52" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B19" s="211" t="s">
+      <c r="B19" s="203" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="212"/>
-      <c r="D19" s="212"/>
-      <c r="E19" s="213"/>
+      <c r="C19" s="204"/>
+      <c r="D19" s="204"/>
+      <c r="E19" s="205"/>
     </row>
     <row r="20" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B20" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="214" t="s">
+      <c r="C20" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="215"/>
-      <c r="E20" s="216"/>
+      <c r="D20" s="207"/>
+      <c r="E20" s="208"/>
     </row>
     <row r="21" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1">
       <c r="B21" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="202" t="s">
+      <c r="C21" s="220" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="203"/>
-      <c r="E21" s="204"/>
+      <c r="D21" s="221"/>
+      <c r="E21" s="222"/>
     </row>
     <row r="22" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1">
       <c r="B22" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="202" t="s">
+      <c r="C22" s="220" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="203"/>
-      <c r="E22" s="204"/>
+      <c r="D22" s="221"/>
+      <c r="E22" s="222"/>
     </row>
     <row r="23" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1">
       <c r="B23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="202" t="s">
+      <c r="C23" s="220" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="203"/>
-      <c r="E23" s="204"/>
+      <c r="D23" s="221"/>
+      <c r="E23" s="222"/>
     </row>
     <row r="24" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B24" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="202" t="s">
+      <c r="C24" s="220" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="203"/>
-      <c r="E24" s="204"/>
+      <c r="D24" s="221"/>
+      <c r="E24" s="222"/>
     </row>
     <row r="25" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B25" s="54"/>
@@ -7769,31 +7779,31 @@
       <c r="B26" s="45"/>
     </row>
     <row r="27" spans="1:8" s="52" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B27" s="211" t="s">
+      <c r="B27" s="203" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="212"/>
-      <c r="D27" s="212"/>
-      <c r="E27" s="213"/>
+      <c r="C27" s="204"/>
+      <c r="D27" s="204"/>
+      <c r="E27" s="205"/>
     </row>
     <row r="28" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B28" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="214" t="s">
+      <c r="C28" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="215"/>
-      <c r="E28" s="216"/>
+      <c r="D28" s="207"/>
+      <c r="E28" s="208"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1">
       <c r="A29" s="32"/>
-      <c r="B29" s="208" t="s">
+      <c r="B29" s="224" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="209"/>
-      <c r="D29" s="209"/>
-      <c r="E29" s="210"/>
+      <c r="C29" s="225"/>
+      <c r="D29" s="225"/>
+      <c r="E29" s="226"/>
       <c r="F29" s="52"/>
       <c r="G29" s="52"/>
     </row>
@@ -7802,11 +7812,11 @@
       <c r="B30" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="198" t="s">
+      <c r="C30" s="197" t="s">
         <v>192</v>
       </c>
-      <c r="D30" s="199"/>
-      <c r="E30" s="200"/>
+      <c r="D30" s="198"/>
+      <c r="E30" s="199"/>
       <c r="F30" s="52"/>
       <c r="G30" s="52"/>
     </row>
@@ -7815,11 +7825,11 @@
       <c r="B31" s="166" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="198" t="s">
+      <c r="C31" s="197" t="s">
         <v>193</v>
       </c>
-      <c r="D31" s="199"/>
-      <c r="E31" s="200"/>
+      <c r="D31" s="198"/>
+      <c r="E31" s="199"/>
       <c r="F31" s="52"/>
       <c r="G31" s="52"/>
     </row>
@@ -7828,11 +7838,11 @@
       <c r="B32" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="198" t="s">
+      <c r="C32" s="197" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="199"/>
-      <c r="E32" s="200"/>
+      <c r="D32" s="198"/>
+      <c r="E32" s="199"/>
       <c r="F32" s="52"/>
       <c r="G32" s="52"/>
     </row>
@@ -7841,11 +7851,11 @@
       <c r="B33" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="198" t="s">
+      <c r="C33" s="197" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="199"/>
-      <c r="E33" s="200"/>
+      <c r="D33" s="198"/>
+      <c r="E33" s="199"/>
       <c r="F33" s="52"/>
       <c r="G33" s="52"/>
     </row>
@@ -7854,174 +7864,174 @@
       <c r="B34" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="198" t="s">
+      <c r="C34" s="197" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="199"/>
-      <c r="E34" s="200"/>
+      <c r="D34" s="198"/>
+      <c r="E34" s="199"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1">
       <c r="A35" s="32"/>
       <c r="B35" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="198" t="s">
+      <c r="C35" s="197" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="199"/>
-      <c r="E35" s="200"/>
+      <c r="D35" s="198"/>
+      <c r="E35" s="199"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" customHeight="1">
       <c r="A36" s="32"/>
-      <c r="B36" s="208" t="s">
+      <c r="B36" s="224" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="209"/>
-      <c r="D36" s="209"/>
-      <c r="E36" s="210"/>
+      <c r="C36" s="225"/>
+      <c r="D36" s="225"/>
+      <c r="E36" s="226"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1">
       <c r="A37" s="32"/>
       <c r="B37" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="198" t="s">
+      <c r="C37" s="197" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="199"/>
-      <c r="E37" s="200"/>
+      <c r="D37" s="198"/>
+      <c r="E37" s="199"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" customHeight="1">
       <c r="A38" s="32"/>
       <c r="B38" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="198" t="s">
+      <c r="C38" s="197" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="199"/>
-      <c r="E38" s="200"/>
+      <c r="D38" s="198"/>
+      <c r="E38" s="199"/>
     </row>
     <row r="39" spans="1:7" ht="17.25" customHeight="1">
       <c r="A39" s="32"/>
       <c r="B39" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="198" t="s">
+      <c r="C39" s="197" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="199"/>
-      <c r="E39" s="200"/>
+      <c r="D39" s="198"/>
+      <c r="E39" s="199"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" customHeight="1">
       <c r="A40" s="32"/>
       <c r="B40" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="198" t="s">
+      <c r="C40" s="197" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="199"/>
-      <c r="E40" s="200"/>
+      <c r="D40" s="198"/>
+      <c r="E40" s="199"/>
     </row>
     <row r="41" spans="1:7" ht="16.5" customHeight="1">
       <c r="A41" s="32"/>
       <c r="B41" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="198" t="s">
+      <c r="C41" s="197" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="199"/>
-      <c r="E41" s="200"/>
+      <c r="D41" s="198"/>
+      <c r="E41" s="199"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" customHeight="1">
       <c r="A42" s="32"/>
       <c r="B42" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="198" t="s">
+      <c r="C42" s="197" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="199"/>
-      <c r="E42" s="200"/>
+      <c r="D42" s="198"/>
+      <c r="E42" s="199"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1">
       <c r="A43" s="32"/>
       <c r="B43" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="198" t="s">
+      <c r="C43" s="197" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="199"/>
-      <c r="E43" s="200"/>
+      <c r="D43" s="198"/>
+      <c r="E43" s="199"/>
     </row>
     <row r="44" spans="1:7" ht="16.5" customHeight="1">
       <c r="A44" s="32"/>
       <c r="B44" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="198" t="s">
+      <c r="C44" s="197" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="199"/>
-      <c r="E44" s="200"/>
+      <c r="D44" s="198"/>
+      <c r="E44" s="199"/>
     </row>
     <row r="45" spans="1:7" ht="16.5" customHeight="1">
       <c r="A45" s="32"/>
       <c r="B45" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="198" t="s">
+      <c r="C45" s="197" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="199"/>
-      <c r="E45" s="200"/>
+      <c r="D45" s="198"/>
+      <c r="E45" s="199"/>
     </row>
     <row r="46" spans="1:7" ht="16.5" customHeight="1">
       <c r="A46" s="32"/>
       <c r="B46" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="198" t="s">
+      <c r="C46" s="197" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="199"/>
-      <c r="E46" s="200"/>
+      <c r="D46" s="198"/>
+      <c r="E46" s="199"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" customHeight="1">
       <c r="A47" s="32"/>
       <c r="B47" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="198" t="s">
+      <c r="C47" s="197" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="199"/>
-      <c r="E47" s="200"/>
+      <c r="D47" s="198"/>
+      <c r="E47" s="199"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" customHeight="1">
       <c r="A48" s="32"/>
       <c r="B48" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="198" t="s">
+      <c r="C48" s="197" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="199"/>
-      <c r="E48" s="200"/>
+      <c r="D48" s="198"/>
+      <c r="E48" s="199"/>
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
       <c r="A49" s="32"/>
       <c r="B49" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="198" t="s">
+      <c r="C49" s="197" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="199"/>
-      <c r="E49" s="200"/>
+      <c r="D49" s="198"/>
+      <c r="E49" s="199"/>
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="52"/>
@@ -8054,23 +8064,23 @@
       <c r="M51" s="33"/>
     </row>
     <row r="52" spans="1:13" s="52" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B52" s="211" t="s">
+      <c r="B52" s="203" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="212"/>
-      <c r="D52" s="212"/>
-      <c r="E52" s="213"/>
+      <c r="C52" s="204"/>
+      <c r="D52" s="204"/>
+      <c r="E52" s="205"/>
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="52"/>
       <c r="B53" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="214" t="s">
+      <c r="C53" s="206" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="215"/>
-      <c r="E53" s="216"/>
+      <c r="D53" s="207"/>
+      <c r="E53" s="208"/>
       <c r="F53" s="52"/>
       <c r="G53" s="52"/>
       <c r="H53" s="52"/>
@@ -8085,132 +8095,132 @@
       <c r="B54" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C54" s="198" t="s">
+      <c r="C54" s="197" t="s">
         <v>75</v>
       </c>
-      <c r="D54" s="199"/>
-      <c r="E54" s="200"/>
+      <c r="D54" s="198"/>
+      <c r="E54" s="199"/>
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
       <c r="A55" s="32"/>
       <c r="B55" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="198" t="s">
+      <c r="C55" s="197" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="199"/>
-      <c r="E55" s="200"/>
+      <c r="D55" s="198"/>
+      <c r="E55" s="199"/>
     </row>
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
       <c r="A56" s="32"/>
       <c r="B56" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="198" t="s">
+      <c r="C56" s="197" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="199"/>
-      <c r="E56" s="200"/>
+      <c r="D56" s="198"/>
+      <c r="E56" s="199"/>
     </row>
     <row r="57" spans="1:13" ht="16.5" customHeight="1">
       <c r="A57" s="32"/>
       <c r="B57" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="198" t="s">
+      <c r="C57" s="197" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="205"/>
-      <c r="E57" s="206"/>
+      <c r="D57" s="201"/>
+      <c r="E57" s="202"/>
     </row>
     <row r="58" spans="1:13" ht="16.5" customHeight="1">
       <c r="A58" s="32"/>
       <c r="B58" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="198" t="s">
+      <c r="C58" s="197" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="205"/>
-      <c r="E58" s="206"/>
+      <c r="D58" s="201"/>
+      <c r="E58" s="202"/>
     </row>
     <row r="59" spans="1:13" ht="16.5" customHeight="1">
       <c r="A59" s="32"/>
       <c r="B59" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="198" t="s">
+      <c r="C59" s="197" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="205"/>
-      <c r="E59" s="206"/>
+      <c r="D59" s="201"/>
+      <c r="E59" s="202"/>
     </row>
     <row r="60" spans="1:13" ht="54" customHeight="1">
       <c r="A60" s="32"/>
       <c r="B60" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="198" t="s">
+      <c r="C60" s="197" t="s">
         <v>107</v>
       </c>
-      <c r="D60" s="205"/>
-      <c r="E60" s="206"/>
+      <c r="D60" s="201"/>
+      <c r="E60" s="202"/>
     </row>
     <row r="61" spans="1:13" ht="16.5" customHeight="1">
       <c r="A61" s="32"/>
       <c r="B61" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="207" t="s">
+      <c r="C61" s="200" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="205"/>
-      <c r="E61" s="206"/>
+      <c r="D61" s="201"/>
+      <c r="E61" s="202"/>
     </row>
     <row r="62" spans="1:13" ht="30" customHeight="1">
       <c r="A62" s="32"/>
       <c r="B62" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="198" t="s">
+      <c r="C62" s="197" t="s">
         <v>56</v>
       </c>
-      <c r="D62" s="205"/>
-      <c r="E62" s="206"/>
+      <c r="D62" s="201"/>
+      <c r="E62" s="202"/>
     </row>
     <row r="63" spans="1:13" ht="16.5" customHeight="1">
       <c r="A63" s="32"/>
       <c r="B63" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="207" t="s">
+      <c r="C63" s="200" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="205"/>
-      <c r="E63" s="206"/>
+      <c r="D63" s="201"/>
+      <c r="E63" s="202"/>
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1">
       <c r="A64" s="32"/>
       <c r="B64" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="207" t="s">
+      <c r="C64" s="200" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="205"/>
-      <c r="E64" s="206"/>
+      <c r="D64" s="201"/>
+      <c r="E64" s="202"/>
     </row>
     <row r="65" spans="1:8" ht="16.5" customHeight="1">
       <c r="A65" s="32"/>
       <c r="B65" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="198" t="s">
+      <c r="C65" s="197" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="199"/>
-      <c r="E65" s="200"/>
+      <c r="D65" s="198"/>
+      <c r="E65" s="199"/>
     </row>
     <row r="66" spans="1:8" ht="16.5" customHeight="1">
       <c r="A66" s="32"/>
@@ -8221,200 +8231,200 @@
     </row>
     <row r="67" spans="1:8" ht="16.5" customHeight="1">
       <c r="A67" s="32"/>
-      <c r="B67" s="201"/>
-      <c r="C67" s="201"/>
-      <c r="D67" s="201"/>
-      <c r="E67" s="201"/>
+      <c r="B67" s="228"/>
+      <c r="C67" s="228"/>
+      <c r="D67" s="228"/>
+      <c r="E67" s="228"/>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
       <c r="H67" s="51"/>
     </row>
     <row r="68" spans="1:8" ht="16.5" customHeight="1">
       <c r="A68" s="32"/>
-      <c r="B68" s="197"/>
-      <c r="C68" s="197"/>
-      <c r="D68" s="197"/>
-      <c r="E68" s="197"/>
+      <c r="B68" s="227"/>
+      <c r="C68" s="227"/>
+      <c r="D68" s="227"/>
+      <c r="E68" s="227"/>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
       <c r="H68" s="51"/>
     </row>
     <row r="69" spans="1:8" ht="16.5" customHeight="1">
       <c r="A69" s="32"/>
-      <c r="B69" s="197"/>
-      <c r="C69" s="197"/>
-      <c r="D69" s="197"/>
-      <c r="E69" s="197"/>
+      <c r="B69" s="227"/>
+      <c r="C69" s="227"/>
+      <c r="D69" s="227"/>
+      <c r="E69" s="227"/>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
       <c r="H69" s="51"/>
     </row>
     <row r="70" spans="1:8" ht="16.5" customHeight="1">
       <c r="A70" s="32"/>
-      <c r="B70" s="197"/>
-      <c r="C70" s="197"/>
-      <c r="D70" s="197"/>
-      <c r="E70" s="197"/>
+      <c r="B70" s="227"/>
+      <c r="C70" s="227"/>
+      <c r="D70" s="227"/>
+      <c r="E70" s="227"/>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
       <c r="H70" s="51"/>
     </row>
     <row r="71" spans="1:8" ht="16.5" customHeight="1">
       <c r="A71" s="32"/>
-      <c r="B71" s="197"/>
-      <c r="C71" s="197"/>
-      <c r="D71" s="197"/>
-      <c r="E71" s="197"/>
+      <c r="B71" s="227"/>
+      <c r="C71" s="227"/>
+      <c r="D71" s="227"/>
+      <c r="E71" s="227"/>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
       <c r="H71" s="51"/>
     </row>
     <row r="72" spans="1:8" ht="16.5" customHeight="1">
       <c r="A72" s="32"/>
-      <c r="B72" s="197"/>
-      <c r="C72" s="197"/>
-      <c r="D72" s="197"/>
-      <c r="E72" s="197"/>
+      <c r="B72" s="227"/>
+      <c r="C72" s="227"/>
+      <c r="D72" s="227"/>
+      <c r="E72" s="227"/>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
       <c r="H72" s="51"/>
     </row>
     <row r="73" spans="1:8" ht="16.5" customHeight="1">
       <c r="A73" s="37"/>
-      <c r="B73" s="197"/>
-      <c r="C73" s="197"/>
-      <c r="D73" s="197"/>
-      <c r="E73" s="197"/>
+      <c r="B73" s="227"/>
+      <c r="C73" s="227"/>
+      <c r="D73" s="227"/>
+      <c r="E73" s="227"/>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
       <c r="H73" s="51"/>
     </row>
     <row r="74" spans="1:8" ht="16.5" customHeight="1">
       <c r="A74" s="32"/>
-      <c r="B74" s="197"/>
-      <c r="C74" s="197"/>
-      <c r="D74" s="197"/>
-      <c r="E74" s="197"/>
+      <c r="B74" s="227"/>
+      <c r="C74" s="227"/>
+      <c r="D74" s="227"/>
+      <c r="E74" s="227"/>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
       <c r="H74" s="51"/>
     </row>
     <row r="75" spans="1:8" ht="16.5" customHeight="1">
       <c r="A75" s="32"/>
-      <c r="B75" s="197"/>
-      <c r="C75" s="197"/>
-      <c r="D75" s="197"/>
-      <c r="E75" s="197"/>
+      <c r="B75" s="227"/>
+      <c r="C75" s="227"/>
+      <c r="D75" s="227"/>
+      <c r="E75" s="227"/>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
       <c r="H75" s="51"/>
     </row>
     <row r="76" spans="1:8" ht="16.5" customHeight="1">
       <c r="A76" s="32"/>
-      <c r="B76" s="197"/>
-      <c r="C76" s="197"/>
-      <c r="D76" s="197"/>
-      <c r="E76" s="197"/>
+      <c r="B76" s="227"/>
+      <c r="C76" s="227"/>
+      <c r="D76" s="227"/>
+      <c r="E76" s="227"/>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
       <c r="H76" s="51"/>
     </row>
     <row r="77" spans="1:8" ht="16.5" customHeight="1">
       <c r="A77" s="32"/>
-      <c r="B77" s="197"/>
-      <c r="C77" s="197"/>
-      <c r="D77" s="197"/>
-      <c r="E77" s="197"/>
+      <c r="B77" s="227"/>
+      <c r="C77" s="227"/>
+      <c r="D77" s="227"/>
+      <c r="E77" s="227"/>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
       <c r="H77" s="51"/>
     </row>
     <row r="78" spans="1:8" ht="16.5" customHeight="1">
       <c r="A78" s="32"/>
-      <c r="B78" s="197"/>
-      <c r="C78" s="197"/>
-      <c r="D78" s="197"/>
-      <c r="E78" s="197"/>
+      <c r="B78" s="227"/>
+      <c r="C78" s="227"/>
+      <c r="D78" s="227"/>
+      <c r="E78" s="227"/>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
       <c r="H78" s="51"/>
     </row>
     <row r="79" spans="1:8" ht="16.5" customHeight="1">
       <c r="A79" s="37"/>
-      <c r="B79" s="197"/>
-      <c r="C79" s="197"/>
-      <c r="D79" s="197"/>
-      <c r="E79" s="197"/>
+      <c r="B79" s="227"/>
+      <c r="C79" s="227"/>
+      <c r="D79" s="227"/>
+      <c r="E79" s="227"/>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
       <c r="H79" s="51"/>
     </row>
     <row r="80" spans="1:8" ht="16.5" customHeight="1">
       <c r="A80" s="37"/>
-      <c r="B80" s="197"/>
-      <c r="C80" s="197"/>
-      <c r="D80" s="197"/>
-      <c r="E80" s="197"/>
+      <c r="B80" s="227"/>
+      <c r="C80" s="227"/>
+      <c r="D80" s="227"/>
+      <c r="E80" s="227"/>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
       <c r="H80" s="51"/>
     </row>
     <row r="81" spans="1:8" ht="16.5" customHeight="1">
       <c r="A81" s="37"/>
-      <c r="B81" s="197"/>
-      <c r="C81" s="197"/>
-      <c r="D81" s="197"/>
-      <c r="E81" s="197"/>
+      <c r="B81" s="227"/>
+      <c r="C81" s="227"/>
+      <c r="D81" s="227"/>
+      <c r="E81" s="227"/>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
       <c r="H81" s="51"/>
     </row>
     <row r="82" spans="1:8" ht="16.5" customHeight="1">
       <c r="A82" s="37"/>
-      <c r="B82" s="197"/>
-      <c r="C82" s="197"/>
-      <c r="D82" s="197"/>
-      <c r="E82" s="197"/>
+      <c r="B82" s="227"/>
+      <c r="C82" s="227"/>
+      <c r="D82" s="227"/>
+      <c r="E82" s="227"/>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
       <c r="H82" s="51"/>
     </row>
     <row r="83" spans="1:8" ht="16.5" customHeight="1">
       <c r="A83" s="37"/>
-      <c r="B83" s="197"/>
-      <c r="C83" s="197"/>
-      <c r="D83" s="197"/>
-      <c r="E83" s="197"/>
+      <c r="B83" s="227"/>
+      <c r="C83" s="227"/>
+      <c r="D83" s="227"/>
+      <c r="E83" s="227"/>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
       <c r="H83" s="51"/>
     </row>
     <row r="84" spans="1:8" ht="16.5" customHeight="1">
       <c r="A84" s="37"/>
-      <c r="B84" s="197"/>
-      <c r="C84" s="197"/>
-      <c r="D84" s="197"/>
-      <c r="E84" s="197"/>
+      <c r="B84" s="227"/>
+      <c r="C84" s="227"/>
+      <c r="D84" s="227"/>
+      <c r="E84" s="227"/>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
       <c r="H84" s="51"/>
     </row>
     <row r="85" spans="1:8" ht="16.5" customHeight="1">
       <c r="A85" s="37"/>
-      <c r="B85" s="197"/>
-      <c r="C85" s="197"/>
-      <c r="D85" s="197"/>
-      <c r="E85" s="197"/>
+      <c r="B85" s="227"/>
+      <c r="C85" s="227"/>
+      <c r="D85" s="227"/>
+      <c r="E85" s="227"/>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
       <c r="H85" s="51"/>
     </row>
     <row r="86" spans="1:8" ht="16.5" customHeight="1">
       <c r="A86" s="37"/>
-      <c r="B86" s="197"/>
-      <c r="C86" s="197"/>
-      <c r="D86" s="197"/>
-      <c r="E86" s="197"/>
+      <c r="B86" s="227"/>
+      <c r="C86" s="227"/>
+      <c r="D86" s="227"/>
+      <c r="E86" s="227"/>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
       <c r="H86" s="51"/>
@@ -8427,40 +8437,27 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C60:E60"/>
@@ -8477,27 +8474,40 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B84:E84"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8513,8 +8523,8 @@
   </sheetPr>
   <dimension ref="A3:Z54"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -8536,22 +8546,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:26" ht="18" customHeight="1">
-      <c r="B3" s="229" t="s">
+      <c r="B3" s="239" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="229"/>
-      <c r="D3" s="229"/>
-      <c r="E3" s="229"/>
-      <c r="F3" s="229"/>
-      <c r="G3" s="229"/>
-      <c r="H3" s="229"/>
-      <c r="I3" s="229"/>
-      <c r="J3" s="229"/>
-      <c r="K3" s="229"/>
-      <c r="L3" s="229"/>
-      <c r="M3" s="229"/>
-      <c r="N3" s="229"/>
-      <c r="O3" s="229"/>
+      <c r="C3" s="239"/>
+      <c r="D3" s="239"/>
+      <c r="E3" s="239"/>
+      <c r="F3" s="239"/>
+      <c r="G3" s="239"/>
+      <c r="H3" s="239"/>
+      <c r="I3" s="239"/>
+      <c r="J3" s="239"/>
+      <c r="K3" s="239"/>
+      <c r="L3" s="239"/>
+      <c r="M3" s="239"/>
+      <c r="N3" s="239"/>
+      <c r="O3" s="239"/>
     </row>
     <row r="4" spans="2:26" ht="11.25" customHeight="1">
       <c r="B4" s="4"/>
@@ -8559,39 +8569,39 @@
     </row>
     <row r="5" spans="2:26" ht="15" customHeight="1"/>
     <row r="6" spans="2:26" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B6" s="231" t="s">
+      <c r="B6" s="230" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="232"/>
-      <c r="D6" s="233"/>
-      <c r="E6" s="234" t="s">
+      <c r="C6" s="231"/>
+      <c r="D6" s="232"/>
+      <c r="E6" s="233" t="s">
         <v>176</v>
       </c>
-      <c r="F6" s="235"/>
-      <c r="G6" s="236"/>
-      <c r="H6" s="230"/>
-      <c r="I6" s="230"/>
+      <c r="F6" s="234"/>
+      <c r="G6" s="235"/>
+      <c r="H6" s="240"/>
+      <c r="I6" s="240"/>
       <c r="O6" s="143"/>
       <c r="Z6" s="3"/>
     </row>
     <row r="7" spans="2:26" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B7" s="231" t="s">
+      <c r="B7" s="230" t="s">
         <v>140</v>
       </c>
-      <c r="C7" s="232"/>
-      <c r="D7" s="233"/>
-      <c r="E7" s="234" t="s">
+      <c r="C7" s="231"/>
+      <c r="D7" s="232"/>
+      <c r="E7" s="233" t="s">
         <v>138</v>
       </c>
-      <c r="F7" s="235"/>
-      <c r="G7" s="236"/>
-      <c r="J7" s="237" t="s">
+      <c r="F7" s="234"/>
+      <c r="G7" s="235"/>
+      <c r="J7" s="229" t="s">
         <v>160</v>
       </c>
-      <c r="K7" s="237"/>
-      <c r="L7" s="237"/>
-      <c r="M7" s="237"/>
-      <c r="N7" s="237"/>
+      <c r="K7" s="229"/>
+      <c r="L7" s="229"/>
+      <c r="M7" s="229"/>
+      <c r="N7" s="229"/>
       <c r="O7" s="164">
         <f>SUM(K13:K49)</f>
         <v>100</v>
@@ -8599,35 +8609,35 @@
       <c r="Z7" s="3"/>
     </row>
     <row r="8" spans="2:26" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B8" s="231" t="s">
+      <c r="B8" s="230" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="232"/>
-      <c r="D8" s="233"/>
-      <c r="E8" s="234" t="s">
+      <c r="C8" s="231"/>
+      <c r="D8" s="232"/>
+      <c r="E8" s="233" t="s">
         <v>175</v>
       </c>
-      <c r="F8" s="235"/>
-      <c r="G8" s="236"/>
-      <c r="J8" s="237" t="s">
+      <c r="F8" s="234"/>
+      <c r="G8" s="235"/>
+      <c r="J8" s="229" t="s">
         <v>161</v>
       </c>
-      <c r="K8" s="237"/>
-      <c r="L8" s="237"/>
-      <c r="M8" s="237"/>
-      <c r="N8" s="237"/>
+      <c r="K8" s="229"/>
+      <c r="L8" s="229"/>
+      <c r="M8" s="229"/>
+      <c r="N8" s="229"/>
       <c r="O8" s="164">
         <f>SUM(N13:N49)</f>
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="Z8" s="3"/>
     </row>
     <row r="9" spans="2:26" s="5" customFormat="1" ht="27.75" customHeight="1">
-      <c r="B9" s="231" t="s">
+      <c r="B9" s="230" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="232"/>
-      <c r="D9" s="233"/>
+      <c r="C9" s="231"/>
+      <c r="D9" s="232"/>
       <c r="E9" s="126">
         <v>42310</v>
       </c>
@@ -8642,16 +8652,16 @@
       <c r="Z9" s="3"/>
     </row>
     <row r="10" spans="2:26" s="5" customFormat="1" ht="15" customHeight="1">
-      <c r="B10" s="231" t="s">
+      <c r="B10" s="230" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="232"/>
-      <c r="D10" s="233"/>
-      <c r="E10" s="238" t="s">
+      <c r="C10" s="231"/>
+      <c r="D10" s="232"/>
+      <c r="E10" s="236" t="s">
         <v>197</v>
       </c>
-      <c r="F10" s="239"/>
-      <c r="G10" s="240"/>
+      <c r="F10" s="237"/>
+      <c r="G10" s="238"/>
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="2:26" s="17" customFormat="1" ht="15" customHeight="1">
@@ -9916,10 +9926,18 @@
       <c r="K40" s="124">
         <v>4</v>
       </c>
-      <c r="L40" s="167"/>
-      <c r="M40" s="167"/>
-      <c r="N40" s="124"/>
-      <c r="O40" s="125"/>
+      <c r="L40" s="167">
+        <v>42319</v>
+      </c>
+      <c r="M40" s="167">
+        <v>42319</v>
+      </c>
+      <c r="N40" s="124">
+        <v>4</v>
+      </c>
+      <c r="O40" s="125" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="41" spans="1:15" s="121" customFormat="1" ht="32.1" customHeight="1">
       <c r="A41" s="123"/>
@@ -9954,10 +9972,18 @@
       <c r="K41" s="124">
         <v>4</v>
       </c>
-      <c r="L41" s="167"/>
-      <c r="M41" s="167"/>
-      <c r="N41" s="124"/>
-      <c r="O41" s="125"/>
+      <c r="L41" s="167">
+        <v>42319</v>
+      </c>
+      <c r="M41" s="167">
+        <v>42319</v>
+      </c>
+      <c r="N41" s="124">
+        <v>4</v>
+      </c>
+      <c r="O41" s="125" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="42" spans="1:15" s="121" customFormat="1" ht="32.1" customHeight="1">
       <c r="A42" s="123"/>
@@ -9992,10 +10018,18 @@
       <c r="K42" s="124">
         <v>2</v>
       </c>
-      <c r="L42" s="167"/>
-      <c r="M42" s="167"/>
-      <c r="N42" s="124"/>
-      <c r="O42" s="125"/>
+      <c r="L42" s="167">
+        <v>42320</v>
+      </c>
+      <c r="M42" s="167">
+        <v>42320</v>
+      </c>
+      <c r="N42" s="124">
+        <v>2</v>
+      </c>
+      <c r="O42" s="125" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="43" spans="1:15" s="121" customFormat="1" ht="32.1" customHeight="1">
       <c r="A43" s="123"/>
@@ -10030,10 +10064,18 @@
       <c r="K43" s="124">
         <v>3</v>
       </c>
-      <c r="L43" s="167"/>
-      <c r="M43" s="167"/>
-      <c r="N43" s="124"/>
-      <c r="O43" s="125"/>
+      <c r="L43" s="167">
+        <v>42320</v>
+      </c>
+      <c r="M43" s="167">
+        <v>42320</v>
+      </c>
+      <c r="N43" s="124">
+        <v>3</v>
+      </c>
+      <c r="O43" s="125" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="44" spans="1:15" s="121" customFormat="1" ht="32.1" customHeight="1">
       <c r="A44" s="123"/>
@@ -10068,10 +10110,18 @@
       <c r="K44" s="124">
         <v>3</v>
       </c>
-      <c r="L44" s="167"/>
-      <c r="M44" s="167"/>
-      <c r="N44" s="124"/>
-      <c r="O44" s="125"/>
+      <c r="L44" s="167">
+        <v>42320</v>
+      </c>
+      <c r="M44" s="167">
+        <v>42320</v>
+      </c>
+      <c r="N44" s="124">
+        <v>3</v>
+      </c>
+      <c r="O44" s="125" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="45" spans="1:15" s="121" customFormat="1" ht="32.1" customHeight="1">
       <c r="A45" s="123"/>
@@ -10291,12 +10341,6 @@
     <row r="54" spans="1:15" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E10:G10"/>
     <mergeCell ref="B3:O3"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="B6:D6"/>
@@ -10304,6 +10348,12 @@
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="J7:N7"/>
     <mergeCell ref="E7:G7"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10350,11 +10400,11 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="5" ySplit="4" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="5" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="11.25"/>
@@ -11898,9 +11948,12 @@
         <f>VLOOKUP(A32,Planificación!B$13:N$49,9,FALSE)</f>
         <v>42319</v>
       </c>
-      <c r="M32" s="170"/>
+      <c r="M32" s="170">
+        <f>VLOOKUP(A32,Planificación!B$13:N$49,12,FALSE)</f>
+        <v>42319</v>
+      </c>
       <c r="N32" s="190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="191" t="s">
         <v>198</v>
@@ -11949,9 +12002,12 @@
         <f>VLOOKUP(A33,Planificación!B$13:N$49,9,FALSE)</f>
         <v>42319</v>
       </c>
-      <c r="M33" s="170"/>
+      <c r="M33" s="170">
+        <f>VLOOKUP(A33,Planificación!B$13:N$49,12,FALSE)</f>
+        <v>42319</v>
+      </c>
       <c r="N33" s="190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33" s="191" t="s">
         <v>198</v>
@@ -12000,9 +12056,12 @@
         <f>VLOOKUP(A34,Planificación!B$13:N$49,9,FALSE)</f>
         <v>42320</v>
       </c>
-      <c r="M34" s="170"/>
+      <c r="M34" s="170">
+        <f>VLOOKUP(A34,Planificación!B$13:N$49,12,FALSE)</f>
+        <v>42320</v>
+      </c>
       <c r="N34" s="190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O34" s="191" t="s">
         <v>198</v>
@@ -12051,9 +12110,12 @@
         <f>VLOOKUP(A35,Planificación!B$13:N$49,9,FALSE)</f>
         <v>42320</v>
       </c>
-      <c r="M35" s="170"/>
+      <c r="M35" s="170">
+        <f>VLOOKUP(A35,Planificación!B$13:N$49,12,FALSE)</f>
+        <v>42320</v>
+      </c>
       <c r="N35" s="190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O35" s="191" t="s">
         <v>198</v>
@@ -12102,9 +12164,12 @@
         <f>VLOOKUP(A36,Planificación!B$13:N$49,9,FALSE)</f>
         <v>42320</v>
       </c>
-      <c r="M36" s="170"/>
+      <c r="M36" s="170">
+        <f>VLOOKUP(A36,Planificación!B$13:N$49,12,FALSE)</f>
+        <v>42320</v>
+      </c>
       <c r="N36" s="190">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O36" s="191" t="s">
         <v>198</v>
@@ -12425,7 +12490,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H41">
       <formula1>TiposNC</formula1>
     </dataValidation>
@@ -12449,8 +12514,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A2:P62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M59" sqref="M59"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -12466,15 +12531,15 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="C2" s="250" t="s">
+      <c r="C2" s="260" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="250"/>
-      <c r="E2" s="250"/>
-      <c r="F2" s="250"/>
-      <c r="G2" s="250"/>
-      <c r="H2" s="250"/>
-      <c r="I2" s="250"/>
+      <c r="D2" s="260"/>
+      <c r="E2" s="260"/>
+      <c r="F2" s="260"/>
+      <c r="G2" s="260"/>
+      <c r="H2" s="260"/>
+      <c r="I2" s="260"/>
       <c r="J2" s="146"/>
       <c r="K2" s="146"/>
       <c r="L2" s="146"/>
@@ -12484,65 +12549,65 @@
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="C4" s="244" t="s">
+      <c r="C4" s="257" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="244"/>
-      <c r="E4" s="245" t="str">
+      <c r="D4" s="257"/>
+      <c r="E4" s="247" t="str">
         <f>IF(Planificación!E6&lt;&gt;"",Planificación!E6,"")</f>
         <v>Roger Apaéstegui Ortega</v>
       </c>
-      <c r="F4" s="246"/>
-      <c r="G4" s="246"/>
-      <c r="H4" s="246"/>
-      <c r="I4" s="247"/>
+      <c r="F4" s="248"/>
+      <c r="G4" s="248"/>
+      <c r="H4" s="248"/>
+      <c r="I4" s="249"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="C5" s="248" t="str">
+      <c r="C5" s="258" t="str">
         <f>Planificación!B7</f>
         <v>Analista de Calidad</v>
       </c>
-      <c r="D5" s="249"/>
-      <c r="E5" s="245" t="str">
+      <c r="D5" s="259"/>
+      <c r="E5" s="247" t="str">
         <f>IF(Planificación!E7&lt;&gt;"",Planificación!E7,"")</f>
         <v>Julio Leonardo Paredes</v>
       </c>
-      <c r="F5" s="246"/>
-      <c r="G5" s="246"/>
-      <c r="H5" s="246"/>
-      <c r="I5" s="247"/>
+      <c r="F5" s="248"/>
+      <c r="G5" s="248"/>
+      <c r="H5" s="248"/>
+      <c r="I5" s="249"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="11"/>
-      <c r="C6" s="252" t="s">
+      <c r="C6" s="245" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="253"/>
-      <c r="E6" s="245" t="str">
+      <c r="D6" s="246"/>
+      <c r="E6" s="247" t="str">
         <f>IF(Planificación!E8&lt;&gt;"",Planificación!E8,"")</f>
         <v>Julio Leonardo Paredes,  Roger Apaéstegui Ortega</v>
       </c>
-      <c r="F6" s="246"/>
-      <c r="G6" s="246"/>
-      <c r="H6" s="246"/>
-      <c r="I6" s="247"/>
+      <c r="F6" s="248"/>
+      <c r="G6" s="248"/>
+      <c r="H6" s="248"/>
+      <c r="I6" s="249"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="24" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="C7" s="255" t="s">
+      <c r="C7" s="251" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="255"/>
-      <c r="E7" s="256">
+      <c r="D7" s="251"/>
+      <c r="E7" s="252">
         <f>IF(Planificación!E9&lt;&gt;"",Planificación!E9,"")</f>
         <v>42310</v>
       </c>
-      <c r="F7" s="257"/>
-      <c r="G7" s="258" t="s">
+      <c r="F7" s="253"/>
+      <c r="G7" s="254" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="259"/>
+      <c r="H7" s="255"/>
       <c r="I7" s="97">
         <f>IF(Planificación!G9&lt;&gt;"",Planificación!G9,"")</f>
         <v>42324</v>
@@ -12550,24 +12615,24 @@
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="C8" s="255" t="s">
+      <c r="C8" s="251" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="260"/>
-      <c r="E8" s="245" t="str">
+      <c r="D8" s="256"/>
+      <c r="E8" s="247" t="str">
         <f>IF(Planificación!E10&lt;&gt;"",Planificación!E10,"")</f>
         <v>NOVIEMBRE</v>
       </c>
-      <c r="F8" s="246"/>
-      <c r="G8" s="246"/>
-      <c r="H8" s="246"/>
-      <c r="I8" s="247"/>
+      <c r="F8" s="248"/>
+      <c r="G8" s="248"/>
+      <c r="H8" s="248"/>
+      <c r="I8" s="249"/>
     </row>
     <row r="13" spans="1:12" ht="15">
-      <c r="C13" s="254" t="s">
+      <c r="C13" s="250" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="254"/>
+      <c r="D13" s="250"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -12588,7 +12653,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="148">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -12596,7 +12661,7 @@
         <v>41</v>
       </c>
       <c r="D16" s="149">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="17" spans="3:14">
@@ -12605,7 +12670,7 @@
       </c>
       <c r="D17" s="98">
         <f>(D16/(IF(D14=0,1,D14)))</f>
-        <v>0.8666666666666667</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="18" spans="3:14">
@@ -12614,7 +12679,7 @@
       </c>
       <c r="D18" s="98">
         <f>1-D17</f>
-        <v>0.1333333333333333</v>
+        <v>9.9999999999999978E-2</v>
       </c>
     </row>
     <row r="19" spans="3:14">
@@ -12649,10 +12714,10 @@
       <c r="E24" s="9"/>
     </row>
     <row r="26" spans="3:14" ht="15" customHeight="1">
-      <c r="C26" s="251" t="s">
+      <c r="C26" s="244" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="251"/>
+      <c r="D26" s="244"/>
     </row>
     <row r="27" spans="3:14">
       <c r="C27" s="30" t="s">
@@ -12726,10 +12791,10 @@
       </c>
     </row>
     <row r="40" spans="3:16" ht="15">
-      <c r="C40" s="251" t="s">
+      <c r="C40" s="244" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="251"/>
+      <c r="D40" s="244"/>
       <c r="P40" s="144"/>
     </row>
     <row r="41" spans="3:16">
@@ -12747,7 +12812,7 @@
       </c>
       <c r="D42" s="109">
         <f>Planificación!O8</f>
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="3:16">
@@ -12756,14 +12821,14 @@
       </c>
       <c r="D43" s="109">
         <f>D42</f>
-        <v>60</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="3:4" ht="15">
-      <c r="C57" s="251" t="s">
+      <c r="C57" s="244" t="s">
         <v>119</v>
       </c>
-      <c r="D57" s="251"/>
+      <c r="D57" s="244"/>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="30" t="s">
@@ -12811,6 +12876,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="C2:I2"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:I6"/>
@@ -12822,11 +12892,6 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="C2:I2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Herramienta Gestión de Aseguramiento de Calidad
</commit_message>
<xml_diff>
--- a/Area_de_Proceso-_PPQA/HGQA/HGQA_V1.0_2015.xlsx
+++ b/Area_de_Proceso-_PPQA/HGQA/HGQA_V1.0_2015.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thefa\Documents\GitHub\UTP-GPS-ALARM\Area_de_Proceso-_PPQA\HGQA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UTP-GPS-ALARM\UTP-GPS-ALARM\Area_de_Proceso-_PPQA\HGQA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="14250" windowHeight="5730" tabRatio="642" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="14250" windowHeight="5730" tabRatio="642" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Historial de Revisiones" sheetId="14" r:id="rId1"/>
@@ -782,13 +782,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_)"/>
   </numFmts>
-  <fonts count="66">
+  <fonts count="65">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1146,13 +1146,6 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2331,13 +2324,13 @@
     <xf numFmtId="0" fontId="59" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="60" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="62" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2371,58 +2364,58 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="24" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="63" fillId="24" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="62" fillId="24" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="24" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="24" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="24" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="24" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="11" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="11" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="11" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="11" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="63" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="29" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="63" fillId="0" borderId="10" xfId="39" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2440,10 +2433,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="65" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="15" fontId="64" fillId="0" borderId="10" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2490,22 +2483,22 @@
     <xf numFmtId="0" fontId="49" fillId="0" borderId="39" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="39" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="39" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="39" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="39" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="65" fillId="0" borderId="39" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="64" fillId="0" borderId="39" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="15" fontId="65" fillId="0" borderId="39" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="15" fontId="64" fillId="0" borderId="39" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="64" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="63" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -2535,131 +2528,136 @@
     <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="43" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="60" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="32" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="36" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="32" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="32" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="32" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="36" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="11" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="30" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="29" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -2672,14 +2670,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="44" fillId="24" borderId="31" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -2692,6 +2682,34 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="25" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="55" fillId="25" borderId="10" xfId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2703,18 +2721,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="30" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="24" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="52" fillId="25" borderId="10" xfId="32" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -2743,21 +2749,8 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="10" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="11" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="25" borderId="29" xfId="39" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="24" borderId="0" xfId="32" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="36" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="53">
@@ -2779,7 +2772,7 @@
     <cellStyle name="60% - Énfasis4" xfId="16" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="17" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="18" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="19" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="19" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="20" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Cancel" xfId="21"/>
     <cellStyle name="Celda de comprobación" xfId="22" builtinId="23" customBuiltin="1"/>
@@ -2834,7 +2827,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -2870,7 +2863,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2893,7 +2885,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2983,7 +2975,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-1E45-479F-AB83-77D83B7E851D}"/>
               </c:ext>
@@ -3028,7 +3020,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-EC92-482A-AE00-7DAF384C4D3C}"/>
               </c:ext>
@@ -3057,7 +3049,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -3080,10 +3072,8 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3115,7 +3105,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-EC92-482A-AE00-7DAF384C4D3C}"/>
             </c:ext>
@@ -3141,7 +3131,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3164,7 +3153,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3199,7 +3188,7 @@
           <a:cs typeface="+mn-cs"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3211,7 +3200,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3247,7 +3236,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3270,7 +3258,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3360,7 +3348,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-9B85-4785-897E-BF8A635C112A}"/>
               </c:ext>
@@ -3405,7 +3393,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-0716-432A-8A0E-B7A5A8092E4A}"/>
               </c:ext>
@@ -3450,7 +3438,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-0716-432A-8A0E-B7A5A8092E4A}"/>
               </c:ext>
@@ -3495,7 +3483,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-0716-432A-8A0E-B7A5A8092E4A}"/>
               </c:ext>
@@ -3540,7 +3528,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-0716-432A-8A0E-B7A5A8092E4A}"/>
               </c:ext>
@@ -3585,7 +3573,7 @@
               </a:effectLst>
               <a:sp3d/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-9B85-4785-897E-BF8A635C112A}"/>
               </c:ext>
@@ -3647,7 +3635,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-0716-432A-8A0E-B7A5A8092E4A}"/>
             </c:ext>
@@ -3705,7 +3693,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3740,7 +3728,7 @@
           <a:cs typeface="+mn-cs"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3752,7 +3740,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -3818,7 +3806,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3867,7 +3855,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-D90A-429B-8317-E4DDE4E6EB04}"/>
               </c:ext>
@@ -3895,7 +3883,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3906,9 +3894,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
@@ -3942,7 +3929,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-D90A-429B-8317-E4DDE4E6EB04}"/>
             </c:ext>
@@ -3958,11 +3945,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="277321160"/>
-        <c:axId val="277321944"/>
+        <c:axId val="347543304"/>
+        <c:axId val="347541344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="277321160"/>
+        <c:axId val="347543304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3999,10 +3986,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277321944"/>
+        <c:crossAx val="347541344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4012,7 +3999,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277321944"/>
+        <c:axId val="347541344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4057,10 +4044,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277321160"/>
+        <c:crossAx val="347543304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4074,7 +4061,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4097,7 +4083,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4132,7 +4118,7 @@
           <a:cs typeface="+mn-cs"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4144,7 +4130,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -4180,7 +4166,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4203,7 +4188,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4327,7 +4312,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7ADE-45C5-8A1C-7D75887A8429}"/>
             </c:ext>
@@ -4396,7 +4381,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7ADE-45C5-8A1C-7D75887A8429}"/>
             </c:ext>
@@ -4465,7 +4450,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7ADE-45C5-8A1C-7D75887A8429}"/>
             </c:ext>
@@ -4481,12 +4466,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="277323120"/>
-        <c:axId val="277323904"/>
+        <c:axId val="347543696"/>
+        <c:axId val="347538992"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="277323120"/>
+        <c:axId val="347543696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4515,7 +4500,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4538,7 +4522,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-PE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4573,10 +4557,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277323904"/>
+        <c:crossAx val="347538992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4586,7 +4570,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="277323904"/>
+        <c:axId val="347538992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4659,7 +4643,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-PE"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -4688,10 +4672,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="277323120"/>
+        <c:crossAx val="347543696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4705,7 +4689,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4728,7 +4711,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4763,7 +4746,7 @@
           <a:cs typeface="+mn-cs"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6837,6 +6820,79 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1707573</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1032196</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="533400" y="180975"/>
+          <a:ext cx="1374198" cy="1003621"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -6886,7 +6942,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7549,8 +7605,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:M87"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61:E61"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -7564,25 +7620,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="56" customFormat="1" ht="12" customHeight="1"/>
-    <row r="2" spans="1:8" s="56" customFormat="1" ht="48.75" customHeight="1">
+    <row r="2" spans="1:8" s="56" customFormat="1" ht="81.75" customHeight="1">
       <c r="A2" s="34"/>
       <c r="B2" s="57"/>
-      <c r="C2" s="209" t="s">
+      <c r="C2" s="260" t="s">
         <v>190</v>
       </c>
-      <c r="D2" s="210"/>
-      <c r="E2" s="211"/>
+      <c r="D2" s="217"/>
+      <c r="E2" s="218"/>
     </row>
     <row r="3" spans="1:8" s="56" customFormat="1">
       <c r="A3" s="34"/>
       <c r="B3" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="217" t="s">
+      <c r="C3" s="224" t="s">
         <v>191</v>
       </c>
-      <c r="D3" s="218"/>
-      <c r="E3" s="219"/>
+      <c r="D3" s="225"/>
+      <c r="E3" s="226"/>
     </row>
     <row r="4" spans="1:8" s="56" customFormat="1" ht="21.75" customHeight="1">
       <c r="A4" s="34"/>
@@ -7594,12 +7650,12 @@
     </row>
     <row r="5" spans="1:8" ht="24.75" customHeight="1">
       <c r="A5" s="34"/>
-      <c r="B5" s="212" t="s">
+      <c r="B5" s="219" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="213"/>
-      <c r="D5" s="213"/>
-      <c r="E5" s="214"/>
+      <c r="C5" s="220"/>
+      <c r="D5" s="220"/>
+      <c r="E5" s="221"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="34"/>
@@ -7622,10 +7678,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="86"/>
-      <c r="D8" s="215" t="s">
+      <c r="D8" s="222" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="216"/>
+      <c r="E8" s="223"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="34"/>
@@ -7640,10 +7696,10 @@
         <v>93</v>
       </c>
       <c r="C10" s="56"/>
-      <c r="D10" s="223" t="s">
+      <c r="D10" s="227" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="223"/>
+      <c r="E10" s="227"/>
     </row>
     <row r="11" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A11" s="34"/>
@@ -7658,10 +7714,10 @@
         <v>93</v>
       </c>
       <c r="C12" s="56"/>
-      <c r="D12" s="223" t="s">
+      <c r="D12" s="227" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="223"/>
+      <c r="E12" s="227"/>
     </row>
     <row r="13" spans="1:8" ht="9.9499999999999993" customHeight="1">
       <c r="A13" s="34"/>
@@ -7676,10 +7732,10 @@
         <v>93</v>
       </c>
       <c r="C14" s="56"/>
-      <c r="D14" s="223" t="s">
+      <c r="D14" s="227" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="223"/>
+      <c r="E14" s="227"/>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="32"/>
@@ -7694,10 +7750,10 @@
         <v>93</v>
       </c>
       <c r="C16" s="56"/>
-      <c r="D16" s="223" t="s">
+      <c r="D16" s="227" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="223"/>
+      <c r="E16" s="227"/>
       <c r="H16" s="36"/>
     </row>
     <row r="17" spans="1:8" s="47" customFormat="1" ht="12" customHeight="1">
@@ -7711,62 +7767,62 @@
       <c r="A18" s="32"/>
     </row>
     <row r="19" spans="1:8" s="52" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B19" s="203" t="s">
+      <c r="B19" s="211" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="204"/>
-      <c r="D19" s="204"/>
-      <c r="E19" s="205"/>
+      <c r="C19" s="212"/>
+      <c r="D19" s="212"/>
+      <c r="E19" s="213"/>
     </row>
     <row r="20" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B20" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="206" t="s">
+      <c r="C20" s="214" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="207"/>
-      <c r="E20" s="208"/>
+      <c r="D20" s="215"/>
+      <c r="E20" s="216"/>
     </row>
     <row r="21" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1">
       <c r="B21" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="220" t="s">
+      <c r="C21" s="202" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="221"/>
-      <c r="E21" s="222"/>
+      <c r="D21" s="203"/>
+      <c r="E21" s="204"/>
     </row>
     <row r="22" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1">
       <c r="B22" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="220" t="s">
+      <c r="C22" s="202" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="221"/>
-      <c r="E22" s="222"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="204"/>
     </row>
     <row r="23" spans="1:8" s="52" customFormat="1" ht="12.75" customHeight="1">
       <c r="B23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="C23" s="220" t="s">
+      <c r="C23" s="202" t="s">
         <v>101</v>
       </c>
-      <c r="D23" s="221"/>
-      <c r="E23" s="222"/>
+      <c r="D23" s="203"/>
+      <c r="E23" s="204"/>
     </row>
     <row r="24" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B24" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="220" t="s">
+      <c r="C24" s="202" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="221"/>
-      <c r="E24" s="222"/>
+      <c r="D24" s="203"/>
+      <c r="E24" s="204"/>
     </row>
     <row r="25" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B25" s="54"/>
@@ -7779,31 +7835,31 @@
       <c r="B26" s="45"/>
     </row>
     <row r="27" spans="1:8" s="52" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B27" s="203" t="s">
+      <c r="B27" s="211" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="204"/>
-      <c r="D27" s="204"/>
-      <c r="E27" s="205"/>
+      <c r="C27" s="212"/>
+      <c r="D27" s="212"/>
+      <c r="E27" s="213"/>
     </row>
     <row r="28" spans="1:8" s="52" customFormat="1" ht="13.5" customHeight="1">
       <c r="B28" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C28" s="206" t="s">
+      <c r="C28" s="214" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="207"/>
-      <c r="E28" s="208"/>
+      <c r="D28" s="215"/>
+      <c r="E28" s="216"/>
     </row>
     <row r="29" spans="1:8" ht="12.75" customHeight="1">
       <c r="A29" s="32"/>
-      <c r="B29" s="224" t="s">
+      <c r="B29" s="208" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="225"/>
-      <c r="D29" s="225"/>
-      <c r="E29" s="226"/>
+      <c r="C29" s="209"/>
+      <c r="D29" s="209"/>
+      <c r="E29" s="210"/>
       <c r="F29" s="52"/>
       <c r="G29" s="52"/>
     </row>
@@ -7812,11 +7868,11 @@
       <c r="B30" s="165" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="197" t="s">
+      <c r="C30" s="198" t="s">
         <v>192</v>
       </c>
-      <c r="D30" s="198"/>
-      <c r="E30" s="199"/>
+      <c r="D30" s="199"/>
+      <c r="E30" s="200"/>
       <c r="F30" s="52"/>
       <c r="G30" s="52"/>
     </row>
@@ -7825,11 +7881,11 @@
       <c r="B31" s="166" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="197" t="s">
+      <c r="C31" s="198" t="s">
         <v>193</v>
       </c>
-      <c r="D31" s="198"/>
-      <c r="E31" s="199"/>
+      <c r="D31" s="199"/>
+      <c r="E31" s="200"/>
       <c r="F31" s="52"/>
       <c r="G31" s="52"/>
     </row>
@@ -7838,11 +7894,11 @@
       <c r="B32" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="197" t="s">
+      <c r="C32" s="198" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="198"/>
-      <c r="E32" s="199"/>
+      <c r="D32" s="199"/>
+      <c r="E32" s="200"/>
       <c r="F32" s="52"/>
       <c r="G32" s="52"/>
     </row>
@@ -7851,11 +7907,11 @@
       <c r="B33" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="197" t="s">
+      <c r="C33" s="198" t="s">
         <v>72</v>
       </c>
-      <c r="D33" s="198"/>
-      <c r="E33" s="199"/>
+      <c r="D33" s="199"/>
+      <c r="E33" s="200"/>
       <c r="F33" s="52"/>
       <c r="G33" s="52"/>
     </row>
@@ -7864,174 +7920,174 @@
       <c r="B34" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C34" s="197" t="s">
+      <c r="C34" s="198" t="s">
         <v>73</v>
       </c>
-      <c r="D34" s="198"/>
-      <c r="E34" s="199"/>
+      <c r="D34" s="199"/>
+      <c r="E34" s="200"/>
     </row>
     <row r="35" spans="1:7" ht="16.5" customHeight="1">
       <c r="A35" s="32"/>
       <c r="B35" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="197" t="s">
+      <c r="C35" s="198" t="s">
         <v>74</v>
       </c>
-      <c r="D35" s="198"/>
-      <c r="E35" s="199"/>
+      <c r="D35" s="199"/>
+      <c r="E35" s="200"/>
     </row>
     <row r="36" spans="1:7" ht="16.5" customHeight="1">
       <c r="A36" s="32"/>
-      <c r="B36" s="224" t="s">
+      <c r="B36" s="208" t="s">
         <v>51</v>
       </c>
-      <c r="C36" s="225"/>
-      <c r="D36" s="225"/>
-      <c r="E36" s="226"/>
+      <c r="C36" s="209"/>
+      <c r="D36" s="209"/>
+      <c r="E36" s="210"/>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1">
       <c r="A37" s="32"/>
       <c r="B37" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="197" t="s">
+      <c r="C37" s="198" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="198"/>
-      <c r="E37" s="199"/>
+      <c r="D37" s="199"/>
+      <c r="E37" s="200"/>
     </row>
     <row r="38" spans="1:7" ht="16.5" customHeight="1">
       <c r="A38" s="32"/>
       <c r="B38" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="197" t="s">
+      <c r="C38" s="198" t="s">
         <v>86</v>
       </c>
-      <c r="D38" s="198"/>
-      <c r="E38" s="199"/>
+      <c r="D38" s="199"/>
+      <c r="E38" s="200"/>
     </row>
     <row r="39" spans="1:7" ht="17.25" customHeight="1">
       <c r="A39" s="32"/>
       <c r="B39" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C39" s="197" t="s">
+      <c r="C39" s="198" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="198"/>
-      <c r="E39" s="199"/>
+      <c r="D39" s="199"/>
+      <c r="E39" s="200"/>
     </row>
     <row r="40" spans="1:7" ht="16.5" customHeight="1">
       <c r="A40" s="32"/>
       <c r="B40" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="C40" s="197" t="s">
+      <c r="C40" s="198" t="s">
         <v>116</v>
       </c>
-      <c r="D40" s="198"/>
-      <c r="E40" s="199"/>
+      <c r="D40" s="199"/>
+      <c r="E40" s="200"/>
     </row>
     <row r="41" spans="1:7" ht="16.5" customHeight="1">
       <c r="A41" s="32"/>
       <c r="B41" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="197" t="s">
+      <c r="C41" s="198" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="198"/>
-      <c r="E41" s="199"/>
+      <c r="D41" s="199"/>
+      <c r="E41" s="200"/>
     </row>
     <row r="42" spans="1:7" ht="16.5" customHeight="1">
       <c r="A42" s="32"/>
       <c r="B42" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C42" s="197" t="s">
+      <c r="C42" s="198" t="s">
         <v>104</v>
       </c>
-      <c r="D42" s="198"/>
-      <c r="E42" s="199"/>
+      <c r="D42" s="199"/>
+      <c r="E42" s="200"/>
     </row>
     <row r="43" spans="1:7" ht="16.5" customHeight="1">
       <c r="A43" s="32"/>
       <c r="B43" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C43" s="197" t="s">
+      <c r="C43" s="198" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="198"/>
-      <c r="E43" s="199"/>
+      <c r="D43" s="199"/>
+      <c r="E43" s="200"/>
     </row>
     <row r="44" spans="1:7" ht="16.5" customHeight="1">
       <c r="A44" s="32"/>
       <c r="B44" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="197" t="s">
+      <c r="C44" s="198" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="198"/>
-      <c r="E44" s="199"/>
+      <c r="D44" s="199"/>
+      <c r="E44" s="200"/>
     </row>
     <row r="45" spans="1:7" ht="16.5" customHeight="1">
       <c r="A45" s="32"/>
       <c r="B45" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C45" s="197" t="s">
+      <c r="C45" s="198" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="198"/>
-      <c r="E45" s="199"/>
+      <c r="D45" s="199"/>
+      <c r="E45" s="200"/>
     </row>
     <row r="46" spans="1:7" ht="16.5" customHeight="1">
       <c r="A46" s="32"/>
       <c r="B46" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="197" t="s">
+      <c r="C46" s="198" t="s">
         <v>81</v>
       </c>
-      <c r="D46" s="198"/>
-      <c r="E46" s="199"/>
+      <c r="D46" s="199"/>
+      <c r="E46" s="200"/>
     </row>
     <row r="47" spans="1:7" ht="16.5" customHeight="1">
       <c r="A47" s="32"/>
       <c r="B47" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C47" s="197" t="s">
+      <c r="C47" s="198" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="198"/>
-      <c r="E47" s="199"/>
+      <c r="D47" s="199"/>
+      <c r="E47" s="200"/>
     </row>
     <row r="48" spans="1:7" ht="16.5" customHeight="1">
       <c r="A48" s="32"/>
       <c r="B48" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="C48" s="197" t="s">
+      <c r="C48" s="198" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="198"/>
-      <c r="E48" s="199"/>
+      <c r="D48" s="199"/>
+      <c r="E48" s="200"/>
     </row>
     <row r="49" spans="1:13" ht="16.5" customHeight="1">
       <c r="A49" s="32"/>
       <c r="B49" s="41" t="s">
         <v>117</v>
       </c>
-      <c r="C49" s="197" t="s">
+      <c r="C49" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="D49" s="198"/>
-      <c r="E49" s="199"/>
+      <c r="D49" s="199"/>
+      <c r="E49" s="200"/>
     </row>
     <row r="50" spans="1:13" ht="16.5" customHeight="1">
       <c r="A50" s="52"/>
@@ -8064,23 +8120,23 @@
       <c r="M51" s="33"/>
     </row>
     <row r="52" spans="1:13" s="52" customFormat="1" ht="16.5" customHeight="1">
-      <c r="B52" s="203" t="s">
+      <c r="B52" s="211" t="s">
         <v>54</v>
       </c>
-      <c r="C52" s="204"/>
-      <c r="D52" s="204"/>
-      <c r="E52" s="205"/>
+      <c r="C52" s="212"/>
+      <c r="D52" s="212"/>
+      <c r="E52" s="213"/>
     </row>
     <row r="53" spans="1:13" ht="16.5" customHeight="1">
       <c r="A53" s="52"/>
       <c r="B53" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="206" t="s">
+      <c r="C53" s="214" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="207"/>
-      <c r="E53" s="208"/>
+      <c r="D53" s="215"/>
+      <c r="E53" s="216"/>
       <c r="F53" s="52"/>
       <c r="G53" s="52"/>
       <c r="H53" s="52"/>
@@ -8095,132 +8151,132 @@
       <c r="B54" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C54" s="197" t="s">
+      <c r="C54" s="198" t="s">
         <v>75</v>
       </c>
-      <c r="D54" s="198"/>
-      <c r="E54" s="199"/>
+      <c r="D54" s="199"/>
+      <c r="E54" s="200"/>
     </row>
     <row r="55" spans="1:13" ht="16.5" customHeight="1">
       <c r="A55" s="32"/>
       <c r="B55" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="C55" s="197" t="s">
+      <c r="C55" s="198" t="s">
         <v>87</v>
       </c>
-      <c r="D55" s="198"/>
-      <c r="E55" s="199"/>
+      <c r="D55" s="199"/>
+      <c r="E55" s="200"/>
     </row>
     <row r="56" spans="1:13" ht="16.5" customHeight="1">
       <c r="A56" s="32"/>
       <c r="B56" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C56" s="197" t="s">
+      <c r="C56" s="198" t="s">
         <v>88</v>
       </c>
-      <c r="D56" s="198"/>
-      <c r="E56" s="199"/>
+      <c r="D56" s="199"/>
+      <c r="E56" s="200"/>
     </row>
     <row r="57" spans="1:13" ht="16.5" customHeight="1">
       <c r="A57" s="32"/>
       <c r="B57" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="C57" s="197" t="s">
+      <c r="C57" s="198" t="s">
         <v>106</v>
       </c>
-      <c r="D57" s="201"/>
-      <c r="E57" s="202"/>
+      <c r="D57" s="205"/>
+      <c r="E57" s="206"/>
     </row>
     <row r="58" spans="1:13" ht="16.5" customHeight="1">
       <c r="A58" s="32"/>
       <c r="B58" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="197" t="s">
+      <c r="C58" s="198" t="s">
         <v>92</v>
       </c>
-      <c r="D58" s="201"/>
-      <c r="E58" s="202"/>
+      <c r="D58" s="205"/>
+      <c r="E58" s="206"/>
     </row>
     <row r="59" spans="1:13" ht="16.5" customHeight="1">
       <c r="A59" s="32"/>
       <c r="B59" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="C59" s="197" t="s">
+      <c r="C59" s="198" t="s">
         <v>83</v>
       </c>
-      <c r="D59" s="201"/>
-      <c r="E59" s="202"/>
+      <c r="D59" s="205"/>
+      <c r="E59" s="206"/>
     </row>
     <row r="60" spans="1:13" ht="54" customHeight="1">
       <c r="A60" s="32"/>
       <c r="B60" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="C60" s="197" t="s">
+      <c r="C60" s="198" t="s">
         <v>107</v>
       </c>
-      <c r="D60" s="201"/>
-      <c r="E60" s="202"/>
+      <c r="D60" s="205"/>
+      <c r="E60" s="206"/>
     </row>
     <row r="61" spans="1:13" ht="16.5" customHeight="1">
       <c r="A61" s="32"/>
       <c r="B61" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="C61" s="200" t="s">
+      <c r="C61" s="207" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="201"/>
-      <c r="E61" s="202"/>
+      <c r="D61" s="205"/>
+      <c r="E61" s="206"/>
     </row>
     <row r="62" spans="1:13" ht="30" customHeight="1">
       <c r="A62" s="32"/>
       <c r="B62" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C62" s="197" t="s">
+      <c r="C62" s="198" t="s">
         <v>56</v>
       </c>
-      <c r="D62" s="201"/>
-      <c r="E62" s="202"/>
+      <c r="D62" s="205"/>
+      <c r="E62" s="206"/>
     </row>
     <row r="63" spans="1:13" ht="16.5" customHeight="1">
       <c r="A63" s="32"/>
       <c r="B63" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C63" s="200" t="s">
+      <c r="C63" s="207" t="s">
         <v>61</v>
       </c>
-      <c r="D63" s="201"/>
-      <c r="E63" s="202"/>
+      <c r="D63" s="205"/>
+      <c r="E63" s="206"/>
     </row>
     <row r="64" spans="1:13" ht="16.5" customHeight="1">
       <c r="A64" s="32"/>
       <c r="B64" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C64" s="200" t="s">
+      <c r="C64" s="207" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="201"/>
-      <c r="E64" s="202"/>
+      <c r="D64" s="205"/>
+      <c r="E64" s="206"/>
     </row>
     <row r="65" spans="1:8" ht="16.5" customHeight="1">
       <c r="A65" s="32"/>
       <c r="B65" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="C65" s="197" t="s">
+      <c r="C65" s="198" t="s">
         <v>77</v>
       </c>
-      <c r="D65" s="198"/>
-      <c r="E65" s="199"/>
+      <c r="D65" s="199"/>
+      <c r="E65" s="200"/>
     </row>
     <row r="66" spans="1:8" ht="16.5" customHeight="1">
       <c r="A66" s="32"/>
@@ -8231,200 +8287,200 @@
     </row>
     <row r="67" spans="1:8" ht="16.5" customHeight="1">
       <c r="A67" s="32"/>
-      <c r="B67" s="228"/>
-      <c r="C67" s="228"/>
-      <c r="D67" s="228"/>
-      <c r="E67" s="228"/>
+      <c r="B67" s="201"/>
+      <c r="C67" s="201"/>
+      <c r="D67" s="201"/>
+      <c r="E67" s="201"/>
       <c r="F67" s="51"/>
       <c r="G67" s="51"/>
       <c r="H67" s="51"/>
     </row>
     <row r="68" spans="1:8" ht="16.5" customHeight="1">
       <c r="A68" s="32"/>
-      <c r="B68" s="227"/>
-      <c r="C68" s="227"/>
-      <c r="D68" s="227"/>
-      <c r="E68" s="227"/>
+      <c r="B68" s="197"/>
+      <c r="C68" s="197"/>
+      <c r="D68" s="197"/>
+      <c r="E68" s="197"/>
       <c r="F68" s="51"/>
       <c r="G68" s="51"/>
       <c r="H68" s="51"/>
     </row>
     <row r="69" spans="1:8" ht="16.5" customHeight="1">
       <c r="A69" s="32"/>
-      <c r="B69" s="227"/>
-      <c r="C69" s="227"/>
-      <c r="D69" s="227"/>
-      <c r="E69" s="227"/>
+      <c r="B69" s="197"/>
+      <c r="C69" s="197"/>
+      <c r="D69" s="197"/>
+      <c r="E69" s="197"/>
       <c r="F69" s="51"/>
       <c r="G69" s="51"/>
       <c r="H69" s="51"/>
     </row>
     <row r="70" spans="1:8" ht="16.5" customHeight="1">
       <c r="A70" s="32"/>
-      <c r="B70" s="227"/>
-      <c r="C70" s="227"/>
-      <c r="D70" s="227"/>
-      <c r="E70" s="227"/>
+      <c r="B70" s="197"/>
+      <c r="C70" s="197"/>
+      <c r="D70" s="197"/>
+      <c r="E70" s="197"/>
       <c r="F70" s="51"/>
       <c r="G70" s="51"/>
       <c r="H70" s="51"/>
     </row>
     <row r="71" spans="1:8" ht="16.5" customHeight="1">
       <c r="A71" s="32"/>
-      <c r="B71" s="227"/>
-      <c r="C71" s="227"/>
-      <c r="D71" s="227"/>
-      <c r="E71" s="227"/>
+      <c r="B71" s="197"/>
+      <c r="C71" s="197"/>
+      <c r="D71" s="197"/>
+      <c r="E71" s="197"/>
       <c r="F71" s="51"/>
       <c r="G71" s="51"/>
       <c r="H71" s="51"/>
     </row>
     <row r="72" spans="1:8" ht="16.5" customHeight="1">
       <c r="A72" s="32"/>
-      <c r="B72" s="227"/>
-      <c r="C72" s="227"/>
-      <c r="D72" s="227"/>
-      <c r="E72" s="227"/>
+      <c r="B72" s="197"/>
+      <c r="C72" s="197"/>
+      <c r="D72" s="197"/>
+      <c r="E72" s="197"/>
       <c r="F72" s="51"/>
       <c r="G72" s="51"/>
       <c r="H72" s="51"/>
     </row>
     <row r="73" spans="1:8" ht="16.5" customHeight="1">
       <c r="A73" s="37"/>
-      <c r="B73" s="227"/>
-      <c r="C73" s="227"/>
-      <c r="D73" s="227"/>
-      <c r="E73" s="227"/>
+      <c r="B73" s="197"/>
+      <c r="C73" s="197"/>
+      <c r="D73" s="197"/>
+      <c r="E73" s="197"/>
       <c r="F73" s="51"/>
       <c r="G73" s="51"/>
       <c r="H73" s="51"/>
     </row>
     <row r="74" spans="1:8" ht="16.5" customHeight="1">
       <c r="A74" s="32"/>
-      <c r="B74" s="227"/>
-      <c r="C74" s="227"/>
-      <c r="D74" s="227"/>
-      <c r="E74" s="227"/>
+      <c r="B74" s="197"/>
+      <c r="C74" s="197"/>
+      <c r="D74" s="197"/>
+      <c r="E74" s="197"/>
       <c r="F74" s="51"/>
       <c r="G74" s="51"/>
       <c r="H74" s="51"/>
     </row>
     <row r="75" spans="1:8" ht="16.5" customHeight="1">
       <c r="A75" s="32"/>
-      <c r="B75" s="227"/>
-      <c r="C75" s="227"/>
-      <c r="D75" s="227"/>
-      <c r="E75" s="227"/>
+      <c r="B75" s="197"/>
+      <c r="C75" s="197"/>
+      <c r="D75" s="197"/>
+      <c r="E75" s="197"/>
       <c r="F75" s="51"/>
       <c r="G75" s="51"/>
       <c r="H75" s="51"/>
     </row>
     <row r="76" spans="1:8" ht="16.5" customHeight="1">
       <c r="A76" s="32"/>
-      <c r="B76" s="227"/>
-      <c r="C76" s="227"/>
-      <c r="D76" s="227"/>
-      <c r="E76" s="227"/>
+      <c r="B76" s="197"/>
+      <c r="C76" s="197"/>
+      <c r="D76" s="197"/>
+      <c r="E76" s="197"/>
       <c r="F76" s="51"/>
       <c r="G76" s="51"/>
       <c r="H76" s="51"/>
     </row>
     <row r="77" spans="1:8" ht="16.5" customHeight="1">
       <c r="A77" s="32"/>
-      <c r="B77" s="227"/>
-      <c r="C77" s="227"/>
-      <c r="D77" s="227"/>
-      <c r="E77" s="227"/>
+      <c r="B77" s="197"/>
+      <c r="C77" s="197"/>
+      <c r="D77" s="197"/>
+      <c r="E77" s="197"/>
       <c r="F77" s="51"/>
       <c r="G77" s="51"/>
       <c r="H77" s="51"/>
     </row>
     <row r="78" spans="1:8" ht="16.5" customHeight="1">
       <c r="A78" s="32"/>
-      <c r="B78" s="227"/>
-      <c r="C78" s="227"/>
-      <c r="D78" s="227"/>
-      <c r="E78" s="227"/>
+      <c r="B78" s="197"/>
+      <c r="C78" s="197"/>
+      <c r="D78" s="197"/>
+      <c r="E78" s="197"/>
       <c r="F78" s="51"/>
       <c r="G78" s="51"/>
       <c r="H78" s="51"/>
     </row>
     <row r="79" spans="1:8" ht="16.5" customHeight="1">
       <c r="A79" s="37"/>
-      <c r="B79" s="227"/>
-      <c r="C79" s="227"/>
-      <c r="D79" s="227"/>
-      <c r="E79" s="227"/>
+      <c r="B79" s="197"/>
+      <c r="C79" s="197"/>
+      <c r="D79" s="197"/>
+      <c r="E79" s="197"/>
       <c r="F79" s="51"/>
       <c r="G79" s="51"/>
       <c r="H79" s="51"/>
     </row>
     <row r="80" spans="1:8" ht="16.5" customHeight="1">
       <c r="A80" s="37"/>
-      <c r="B80" s="227"/>
-      <c r="C80" s="227"/>
-      <c r="D80" s="227"/>
-      <c r="E80" s="227"/>
+      <c r="B80" s="197"/>
+      <c r="C80" s="197"/>
+      <c r="D80" s="197"/>
+      <c r="E80" s="197"/>
       <c r="F80" s="51"/>
       <c r="G80" s="51"/>
       <c r="H80" s="51"/>
     </row>
     <row r="81" spans="1:8" ht="16.5" customHeight="1">
       <c r="A81" s="37"/>
-      <c r="B81" s="227"/>
-      <c r="C81" s="227"/>
-      <c r="D81" s="227"/>
-      <c r="E81" s="227"/>
+      <c r="B81" s="197"/>
+      <c r="C81" s="197"/>
+      <c r="D81" s="197"/>
+      <c r="E81" s="197"/>
       <c r="F81" s="51"/>
       <c r="G81" s="51"/>
       <c r="H81" s="51"/>
     </row>
     <row r="82" spans="1:8" ht="16.5" customHeight="1">
       <c r="A82" s="37"/>
-      <c r="B82" s="227"/>
-      <c r="C82" s="227"/>
-      <c r="D82" s="227"/>
-      <c r="E82" s="227"/>
+      <c r="B82" s="197"/>
+      <c r="C82" s="197"/>
+      <c r="D82" s="197"/>
+      <c r="E82" s="197"/>
       <c r="F82" s="51"/>
       <c r="G82" s="51"/>
       <c r="H82" s="51"/>
     </row>
     <row r="83" spans="1:8" ht="16.5" customHeight="1">
       <c r="A83" s="37"/>
-      <c r="B83" s="227"/>
-      <c r="C83" s="227"/>
-      <c r="D83" s="227"/>
-      <c r="E83" s="227"/>
+      <c r="B83" s="197"/>
+      <c r="C83" s="197"/>
+      <c r="D83" s="197"/>
+      <c r="E83" s="197"/>
       <c r="F83" s="51"/>
       <c r="G83" s="51"/>
       <c r="H83" s="51"/>
     </row>
     <row r="84" spans="1:8" ht="16.5" customHeight="1">
       <c r="A84" s="37"/>
-      <c r="B84" s="227"/>
-      <c r="C84" s="227"/>
-      <c r="D84" s="227"/>
-      <c r="E84" s="227"/>
+      <c r="B84" s="197"/>
+      <c r="C84" s="197"/>
+      <c r="D84" s="197"/>
+      <c r="E84" s="197"/>
       <c r="F84" s="51"/>
       <c r="G84" s="51"/>
       <c r="H84" s="51"/>
     </row>
     <row r="85" spans="1:8" ht="16.5" customHeight="1">
       <c r="A85" s="37"/>
-      <c r="B85" s="227"/>
-      <c r="C85" s="227"/>
-      <c r="D85" s="227"/>
-      <c r="E85" s="227"/>
+      <c r="B85" s="197"/>
+      <c r="C85" s="197"/>
+      <c r="D85" s="197"/>
+      <c r="E85" s="197"/>
       <c r="F85" s="51"/>
       <c r="G85" s="51"/>
       <c r="H85" s="51"/>
     </row>
     <row r="86" spans="1:8" ht="16.5" customHeight="1">
       <c r="A86" s="37"/>
-      <c r="B86" s="227"/>
-      <c r="C86" s="227"/>
-      <c r="D86" s="227"/>
-      <c r="E86" s="227"/>
+      <c r="B86" s="197"/>
+      <c r="C86" s="197"/>
+      <c r="D86" s="197"/>
+      <c r="E86" s="197"/>
       <c r="F86" s="51"/>
       <c r="G86" s="51"/>
       <c r="H86" s="51"/>
@@ -8437,27 +8493,40 @@
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="B86:E86"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="B81:E81"/>
-    <mergeCell ref="B82:E82"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="B85:E85"/>
-    <mergeCell ref="B83:E83"/>
-    <mergeCell ref="B84:E84"/>
-    <mergeCell ref="B70:E70"/>
-    <mergeCell ref="C65:E65"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="B67:E67"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D16:E16"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C24:E24"/>
     <mergeCell ref="C60:E60"/>
@@ -8474,45 +8543,33 @@
     <mergeCell ref="C39:E39"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="B70:E70"/>
+    <mergeCell ref="C65:E65"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="B67:E67"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:E69"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="B86:E86"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="B81:E81"/>
+    <mergeCell ref="B82:E82"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="B85:E85"/>
+    <mergeCell ref="B83:E83"/>
+    <mergeCell ref="B84:E84"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8523,7 +8580,7 @@
   </sheetPr>
   <dimension ref="A3:Z54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C37" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
@@ -8546,22 +8603,22 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:26" ht="18" customHeight="1">
-      <c r="B3" s="239" t="s">
+      <c r="B3" s="228" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="239"/>
-      <c r="D3" s="239"/>
-      <c r="E3" s="239"/>
-      <c r="F3" s="239"/>
-      <c r="G3" s="239"/>
-      <c r="H3" s="239"/>
-      <c r="I3" s="239"/>
-      <c r="J3" s="239"/>
-      <c r="K3" s="239"/>
-      <c r="L3" s="239"/>
-      <c r="M3" s="239"/>
-      <c r="N3" s="239"/>
-      <c r="O3" s="239"/>
+      <c r="C3" s="228"/>
+      <c r="D3" s="228"/>
+      <c r="E3" s="228"/>
+      <c r="F3" s="228"/>
+      <c r="G3" s="228"/>
+      <c r="H3" s="228"/>
+      <c r="I3" s="228"/>
+      <c r="J3" s="228"/>
+      <c r="K3" s="228"/>
+      <c r="L3" s="228"/>
+      <c r="M3" s="228"/>
+      <c r="N3" s="228"/>
+      <c r="O3" s="228"/>
     </row>
     <row r="4" spans="2:26" ht="11.25" customHeight="1">
       <c r="B4" s="4"/>
@@ -8579,8 +8636,8 @@
       </c>
       <c r="F6" s="234"/>
       <c r="G6" s="235"/>
-      <c r="H6" s="240"/>
-      <c r="I6" s="240"/>
+      <c r="H6" s="229"/>
+      <c r="I6" s="229"/>
       <c r="O6" s="143"/>
       <c r="Z6" s="3"/>
     </row>
@@ -8595,13 +8652,13 @@
       </c>
       <c r="F7" s="234"/>
       <c r="G7" s="235"/>
-      <c r="J7" s="229" t="s">
+      <c r="J7" s="236" t="s">
         <v>160</v>
       </c>
-      <c r="K7" s="229"/>
-      <c r="L7" s="229"/>
-      <c r="M7" s="229"/>
-      <c r="N7" s="229"/>
+      <c r="K7" s="236"/>
+      <c r="L7" s="236"/>
+      <c r="M7" s="236"/>
+      <c r="N7" s="236"/>
       <c r="O7" s="164">
         <f>SUM(K13:K49)</f>
         <v>100</v>
@@ -8619,13 +8676,13 @@
       </c>
       <c r="F8" s="234"/>
       <c r="G8" s="235"/>
-      <c r="J8" s="229" t="s">
+      <c r="J8" s="236" t="s">
         <v>161</v>
       </c>
-      <c r="K8" s="229"/>
-      <c r="L8" s="229"/>
-      <c r="M8" s="229"/>
-      <c r="N8" s="229"/>
+      <c r="K8" s="236"/>
+      <c r="L8" s="236"/>
+      <c r="M8" s="236"/>
+      <c r="N8" s="236"/>
       <c r="O8" s="164">
         <f>SUM(N13:N49)</f>
         <v>76</v>
@@ -8657,11 +8714,11 @@
       </c>
       <c r="C10" s="231"/>
       <c r="D10" s="232"/>
-      <c r="E10" s="236" t="s">
+      <c r="E10" s="237" t="s">
         <v>197</v>
       </c>
-      <c r="F10" s="237"/>
-      <c r="G10" s="238"/>
+      <c r="F10" s="238"/>
+      <c r="G10" s="239"/>
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="2:26" s="17" customFormat="1" ht="15" customHeight="1">
@@ -10341,6 +10398,12 @@
     <row r="54" spans="1:15" ht="12.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E10:G10"/>
     <mergeCell ref="B3:O3"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="B6:D6"/>
@@ -10348,12 +10411,6 @@
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="J7:N7"/>
     <mergeCell ref="E7:G7"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -10425,22 +10482,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="25" customFormat="1" ht="64.5" customHeight="1" thickBot="1">
-      <c r="A1" s="241" t="s">
+      <c r="A1" s="240" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="242"/>
-      <c r="C1" s="242"/>
-      <c r="D1" s="242"/>
-      <c r="E1" s="242"/>
-      <c r="F1" s="242"/>
-      <c r="G1" s="242"/>
-      <c r="H1" s="242"/>
-      <c r="I1" s="242"/>
-      <c r="J1" s="242"/>
-      <c r="K1" s="242"/>
-      <c r="L1" s="242"/>
-      <c r="M1" s="242"/>
-      <c r="N1" s="243"/>
+      <c r="B1" s="241"/>
+      <c r="C1" s="241"/>
+      <c r="D1" s="241"/>
+      <c r="E1" s="241"/>
+      <c r="F1" s="241"/>
+      <c r="G1" s="241"/>
+      <c r="H1" s="241"/>
+      <c r="I1" s="241"/>
+      <c r="J1" s="241"/>
+      <c r="K1" s="241"/>
+      <c r="L1" s="241"/>
+      <c r="M1" s="241"/>
+      <c r="N1" s="242"/>
     </row>
     <row r="2" spans="1:15" s="25" customFormat="1" ht="11.45" customHeight="1">
       <c r="A2" s="26"/>
@@ -12531,15 +12588,15 @@
   <sheetData>
     <row r="2" spans="1:12" s="1" customFormat="1" ht="17.25" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="C2" s="260" t="s">
+      <c r="C2" s="249" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="260"/>
-      <c r="E2" s="260"/>
-      <c r="F2" s="260"/>
-      <c r="G2" s="260"/>
-      <c r="H2" s="260"/>
-      <c r="I2" s="260"/>
+      <c r="D2" s="249"/>
+      <c r="E2" s="249"/>
+      <c r="F2" s="249"/>
+      <c r="G2" s="249"/>
+      <c r="H2" s="249"/>
+      <c r="I2" s="249"/>
       <c r="J2" s="146"/>
       <c r="K2" s="146"/>
       <c r="L2" s="146"/>
@@ -12549,65 +12606,65 @@
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A4" s="11"/>
-      <c r="C4" s="257" t="s">
+      <c r="C4" s="243" t="s">
         <v>135</v>
       </c>
-      <c r="D4" s="257"/>
-      <c r="E4" s="247" t="str">
+      <c r="D4" s="243"/>
+      <c r="E4" s="244" t="str">
         <f>IF(Planificación!E6&lt;&gt;"",Planificación!E6,"")</f>
         <v>Roger Apaéstegui Ortega</v>
       </c>
-      <c r="F4" s="248"/>
-      <c r="G4" s="248"/>
-      <c r="H4" s="248"/>
-      <c r="I4" s="249"/>
+      <c r="F4" s="245"/>
+      <c r="G4" s="245"/>
+      <c r="H4" s="245"/>
+      <c r="I4" s="246"/>
     </row>
     <row r="5" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A5" s="11"/>
-      <c r="C5" s="258" t="str">
+      <c r="C5" s="247" t="str">
         <f>Planificación!B7</f>
         <v>Analista de Calidad</v>
       </c>
-      <c r="D5" s="259"/>
-      <c r="E5" s="247" t="str">
+      <c r="D5" s="248"/>
+      <c r="E5" s="244" t="str">
         <f>IF(Planificación!E7&lt;&gt;"",Planificación!E7,"")</f>
         <v>Julio Leonardo Paredes</v>
       </c>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="249"/>
+      <c r="F5" s="245"/>
+      <c r="G5" s="245"/>
+      <c r="H5" s="245"/>
+      <c r="I5" s="246"/>
     </row>
     <row r="6" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="11"/>
-      <c r="C6" s="245" t="s">
+      <c r="C6" s="251" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="246"/>
-      <c r="E6" s="247" t="str">
+      <c r="D6" s="252"/>
+      <c r="E6" s="244" t="str">
         <f>IF(Planificación!E8&lt;&gt;"",Planificación!E8,"")</f>
         <v>Julio Leonardo Paredes,  Roger Apaéstegui Ortega</v>
       </c>
-      <c r="F6" s="248"/>
-      <c r="G6" s="248"/>
-      <c r="H6" s="248"/>
-      <c r="I6" s="249"/>
+      <c r="F6" s="245"/>
+      <c r="G6" s="245"/>
+      <c r="H6" s="245"/>
+      <c r="I6" s="246"/>
     </row>
     <row r="7" spans="1:12" s="2" customFormat="1" ht="24" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="C7" s="251" t="s">
+      <c r="C7" s="254" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="251"/>
-      <c r="E7" s="252">
+      <c r="D7" s="254"/>
+      <c r="E7" s="255">
         <f>IF(Planificación!E9&lt;&gt;"",Planificación!E9,"")</f>
         <v>42310</v>
       </c>
-      <c r="F7" s="253"/>
-      <c r="G7" s="254" t="s">
+      <c r="F7" s="256"/>
+      <c r="G7" s="257" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="255"/>
+      <c r="H7" s="258"/>
       <c r="I7" s="97">
         <f>IF(Planificación!G9&lt;&gt;"",Planificación!G9,"")</f>
         <v>42324</v>
@@ -12615,24 +12672,24 @@
     </row>
     <row r="8" spans="1:12" s="2" customFormat="1" ht="12.75" customHeight="1">
       <c r="A8" s="11"/>
-      <c r="C8" s="251" t="s">
+      <c r="C8" s="254" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="256"/>
-      <c r="E8" s="247" t="str">
+      <c r="D8" s="259"/>
+      <c r="E8" s="244" t="str">
         <f>IF(Planificación!E10&lt;&gt;"",Planificación!E10,"")</f>
         <v>NOVIEMBRE</v>
       </c>
-      <c r="F8" s="248"/>
-      <c r="G8" s="248"/>
-      <c r="H8" s="248"/>
-      <c r="I8" s="249"/>
+      <c r="F8" s="245"/>
+      <c r="G8" s="245"/>
+      <c r="H8" s="245"/>
+      <c r="I8" s="246"/>
     </row>
     <row r="13" spans="1:12" ht="15">
-      <c r="C13" s="250" t="s">
+      <c r="C13" s="253" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="250"/>
+      <c r="D13" s="253"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
@@ -12714,10 +12771,10 @@
       <c r="E24" s="9"/>
     </row>
     <row r="26" spans="3:14" ht="15" customHeight="1">
-      <c r="C26" s="244" t="s">
+      <c r="C26" s="250" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="244"/>
+      <c r="D26" s="250"/>
     </row>
     <row r="27" spans="3:14">
       <c r="C27" s="30" t="s">
@@ -12791,10 +12848,10 @@
       </c>
     </row>
     <row r="40" spans="3:16" ht="15">
-      <c r="C40" s="244" t="s">
+      <c r="C40" s="250" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="244"/>
+      <c r="D40" s="250"/>
       <c r="P40" s="144"/>
     </row>
     <row r="41" spans="3:16">
@@ -12825,10 +12882,10 @@
       </c>
     </row>
     <row r="57" spans="3:4" ht="15">
-      <c r="C57" s="244" t="s">
+      <c r="C57" s="250" t="s">
         <v>119</v>
       </c>
-      <c r="D57" s="244"/>
+      <c r="D57" s="250"/>
     </row>
     <row r="58" spans="3:4">
       <c r="C58" s="30" t="s">
@@ -12876,11 +12933,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="C2:I2"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:I6"/>
@@ -12892,6 +12944,11 @@
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="C2:I2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>